<commit_message>
Hawkins graph now Viridis
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/EV data from Hawkins.xlsx
+++ b/chapters/ch08-Transportation/datasets/EV data from Hawkins.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F103C1E-6088-D54F-B9E3-EF69CF5E1102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D17DBDA-A25B-2A4F-9C0B-83863F91C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{586E1F71-0C46-D24B-9AE0-864EA31C6727}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="24660" windowHeight="13280" xr2:uid="{586E1F71-0C46-D24B-9AE0-864EA31C6727}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="1" r:id="rId1"/>
-    <sheet name="Hawkins supplementa information" sheetId="2" r:id="rId2"/>
+    <sheet name="Hawkins supplemental info" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -24,9 +24,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
     <t>EV-Euro</t>
   </si>
@@ -70,18 +68,6 @@
     <t>Life cycle component</t>
   </si>
   <si>
-    <t>Other Powertrain</t>
-  </si>
-  <si>
-    <t>Use Phase, non fuel-related</t>
-  </si>
-  <si>
-    <t>Fuel/Electricity</t>
-  </si>
-  <si>
-    <t>End of Life</t>
-  </si>
-  <si>
     <t>Table S1 -2 Normalized impact scores</t>
   </si>
   <si>
@@ -94,13 +80,22 @@
     <t>Metal Depletion</t>
   </si>
   <si>
-    <t>Tita;</t>
-  </si>
-  <si>
-    <t>EOL</t>
-  </si>
-  <si>
-    <t>Use phase (non-fuel)</t>
+    <t>Other powertrain</t>
+  </si>
+  <si>
+    <t>Use phase</t>
+  </si>
+  <si>
+    <t>Fuel/electricity</t>
+  </si>
+  <si>
+    <t>End of life</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>ICE-Gas</t>
   </si>
 </sst>
 </file>
@@ -275,8 +270,8 @@
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>76800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>179913</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>192613</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -611,271 +606,271 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545E4E2A-C014-C447-B414-163A5DC3E9E2}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" t="str">
-        <f>'Hawkins supplementa information'!A5</f>
+        <f>'Hawkins supplemental info'!A5</f>
         <v>Vehicle types</v>
       </c>
       <c r="B1" t="str">
-        <f>'Hawkins supplementa information'!B5</f>
+        <f>'Hawkins supplemental info'!B5</f>
         <v>Impact</v>
       </c>
       <c r="C1" s="5" t="str">
-        <f>'Hawkins supplementa information'!C6</f>
+        <f>'Hawkins supplemental info'!C6</f>
         <v>Base vehicle</v>
       </c>
       <c r="D1" s="5" t="str">
-        <f>'Hawkins supplementa information'!D6</f>
+        <f>'Hawkins supplemental info'!D6</f>
         <v>Engine</v>
       </c>
       <c r="E1" s="5" t="str">
-        <f>'Hawkins supplementa information'!E6</f>
-        <v>Other Powertrain</v>
+        <f>'Hawkins supplemental info'!E6</f>
+        <v>Other powertrain</v>
       </c>
       <c r="F1" s="5" t="str">
-        <f>'Hawkins supplementa information'!F6</f>
+        <f>'Hawkins supplemental info'!F6</f>
         <v>Battery</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="H1" s="5" t="str">
-        <f>'Hawkins supplementa information'!H6</f>
-        <v>Fuel/Electricity</v>
+        <f>'Hawkins supplemental info'!H6</f>
+        <v>Fuel/electricity</v>
       </c>
       <c r="I1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="4"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="4"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="str">
-        <f>'Hawkins supplementa information'!A7</f>
-        <v>ICEV - Gasoline</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2">
-        <f>'Hawkins supplementa information'!C7</f>
+        <f>'Hawkins supplemental info'!C7</f>
         <v>0.11</v>
       </c>
       <c r="D2">
-        <f>'Hawkins supplementa information'!D7</f>
+        <f>'Hawkins supplemental info'!D7</f>
         <v>0.01</v>
       </c>
       <c r="E2">
-        <f>'Hawkins supplementa information'!E7</f>
+        <f>'Hawkins supplemental info'!E7</f>
         <v>0.02</v>
       </c>
       <c r="F2">
-        <f>'Hawkins supplementa information'!F7</f>
+        <f>'Hawkins supplemental info'!F7</f>
         <v>0</v>
       </c>
       <c r="G2">
-        <f>'Hawkins supplementa information'!G7</f>
+        <f>'Hawkins supplemental info'!G7</f>
         <v>0.03</v>
       </c>
       <c r="H2">
-        <f>'Hawkins supplementa information'!H7</f>
+        <f>'Hawkins supplemental info'!H7</f>
         <v>0.65</v>
       </c>
       <c r="I2">
-        <f>'Hawkins supplementa information'!I7</f>
+        <f>'Hawkins supplemental info'!I7</f>
         <v>0.01</v>
       </c>
       <c r="J2" s="4"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
-        <f>'Hawkins supplementa information'!A8</f>
+        <f>'Hawkins supplemental info'!A8</f>
         <v>EV-Euro</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
       <c r="C3">
-        <f>'Hawkins supplementa information'!C8</f>
+        <f>'Hawkins supplemental info'!C8</f>
         <v>0.11</v>
       </c>
       <c r="D3">
-        <f>'Hawkins supplementa information'!D8</f>
+        <f>'Hawkins supplemental info'!D8</f>
         <v>0.02</v>
       </c>
       <c r="E3">
-        <f>'Hawkins supplementa information'!E8</f>
+        <f>'Hawkins supplemental info'!E8</f>
         <v>0.05</v>
       </c>
       <c r="F3">
-        <f>'Hawkins supplementa information'!F8</f>
+        <f>'Hawkins supplemental info'!F8</f>
         <v>0.1</v>
       </c>
       <c r="G3">
-        <f>'Hawkins supplementa information'!G8</f>
+        <f>'Hawkins supplemental info'!G8</f>
         <v>0.02</v>
       </c>
       <c r="H3">
-        <f>'Hawkins supplementa information'!H8</f>
+        <f>'Hawkins supplemental info'!H8</f>
         <v>0.31</v>
       </c>
       <c r="I3">
-        <f>'Hawkins supplementa information'!I8</f>
+        <f>'Hawkins supplemental info'!I8</f>
         <v>0.01</v>
       </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="str">
-        <f>'Hawkins supplementa information'!A9</f>
+        <f>'Hawkins supplemental info'!A9</f>
         <v>EV-Coal</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
-        <f>'Hawkins supplementa information'!C9</f>
+        <f>'Hawkins supplemental info'!C9</f>
         <v>0.11</v>
       </c>
       <c r="D4">
-        <f>'Hawkins supplementa information'!D9</f>
+        <f>'Hawkins supplemental info'!D9</f>
         <v>0.02</v>
       </c>
       <c r="E4">
-        <f>'Hawkins supplementa information'!E9</f>
+        <f>'Hawkins supplemental info'!E9</f>
         <v>0.05</v>
       </c>
       <c r="F4">
-        <f>'Hawkins supplementa information'!F9</f>
+        <f>'Hawkins supplemental info'!F9</f>
         <v>0.1</v>
       </c>
       <c r="G4">
-        <f>'Hawkins supplementa information'!G9</f>
+        <f>'Hawkins supplemental info'!G9</f>
         <v>0.02</v>
       </c>
       <c r="H4">
-        <f>'Hawkins supplementa information'!H9</f>
+        <f>'Hawkins supplemental info'!H9</f>
         <v>0.68</v>
       </c>
       <c r="I4">
-        <f>'Hawkins supplementa information'!I9</f>
+        <f>'Hawkins supplemental info'!I9</f>
         <v>0.01</v>
       </c>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="str">
-        <f>'Hawkins supplementa information'!A10</f>
-        <v>ICEV - Gasoline</v>
+      <c r="A5" t="s">
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
       </c>
       <c r="C5">
-        <f>'Hawkins supplementa information'!C10</f>
+        <f>'Hawkins supplemental info'!C10</f>
         <v>0.22</v>
       </c>
       <c r="D5">
-        <f>'Hawkins supplementa information'!D10</f>
+        <f>'Hawkins supplemental info'!D10</f>
         <v>0.02</v>
       </c>
       <c r="E5">
-        <f>'Hawkins supplementa information'!E10</f>
+        <f>'Hawkins supplemental info'!E10</f>
         <v>0.05</v>
       </c>
       <c r="F5">
-        <f>'Hawkins supplementa information'!F10</f>
+        <f>'Hawkins supplemental info'!F10</f>
         <v>0</v>
       </c>
       <c r="G5">
-        <f>'Hawkins supplementa information'!G10</f>
+        <f>'Hawkins supplemental info'!G10</f>
         <v>0.03</v>
       </c>
       <c r="H5">
-        <f>'Hawkins supplementa information'!H10</f>
+        <f>'Hawkins supplemental info'!H10</f>
         <v>0.01</v>
       </c>
       <c r="I5">
-        <f>'Hawkins supplementa information'!I10</f>
+        <f>'Hawkins supplemental info'!I10</f>
         <v>0</v>
       </c>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
-        <f>'Hawkins supplementa information'!A11</f>
+        <f>'Hawkins supplemental info'!A11</f>
         <v>EV-Euro</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
       <c r="C6">
-        <f>'Hawkins supplementa information'!C11</f>
+        <f>'Hawkins supplemental info'!C11</f>
         <v>0.22</v>
       </c>
       <c r="D6">
-        <f>'Hawkins supplementa information'!D11</f>
+        <f>'Hawkins supplemental info'!D11</f>
         <v>0.16</v>
       </c>
       <c r="E6">
-        <f>'Hawkins supplementa information'!E11</f>
+        <f>'Hawkins supplemental info'!E11</f>
         <v>0.27</v>
       </c>
       <c r="F6">
-        <f>'Hawkins supplementa information'!F11</f>
+        <f>'Hawkins supplemental info'!F11</f>
         <v>0.26</v>
       </c>
       <c r="G6">
-        <f>'Hawkins supplementa information'!G11</f>
+        <f>'Hawkins supplemental info'!G11</f>
         <v>0.05</v>
       </c>
       <c r="H6">
-        <f>'Hawkins supplementa information'!H11</f>
+        <f>'Hawkins supplemental info'!H11</f>
         <v>0.05</v>
       </c>
       <c r="I6">
-        <f>'Hawkins supplementa information'!I11</f>
+        <f>'Hawkins supplemental info'!I11</f>
         <v>0</v>
       </c>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="str">
-        <f>'Hawkins supplementa information'!A12</f>
+        <f>'Hawkins supplemental info'!A12</f>
         <v>EV-Coal</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
       </c>
       <c r="C7">
-        <f>'Hawkins supplementa information'!C12</f>
+        <f>'Hawkins supplemental info'!C12</f>
         <v>0.22</v>
       </c>
       <c r="D7">
-        <f>'Hawkins supplementa information'!D12</f>
+        <f>'Hawkins supplemental info'!D12</f>
         <v>0.16</v>
       </c>
       <c r="E7">
-        <f>'Hawkins supplementa information'!E12</f>
+        <f>'Hawkins supplemental info'!E12</f>
         <v>0.27</v>
       </c>
       <c r="F7">
-        <f>'Hawkins supplementa information'!F12</f>
+        <f>'Hawkins supplemental info'!F12</f>
         <v>0.26</v>
       </c>
       <c r="G7">
-        <f>'Hawkins supplementa information'!G12</f>
+        <f>'Hawkins supplemental info'!G12</f>
         <v>0.05</v>
       </c>
       <c r="H7">
-        <f>'Hawkins supplementa information'!H12</f>
+        <f>'Hawkins supplemental info'!H12</f>
         <v>0.05</v>
       </c>
       <c r="I7">
-        <f>'Hawkins supplementa information'!I12</f>
+        <f>'Hawkins supplemental info'!I12</f>
         <v>0</v>
       </c>
       <c r="J7" s="4"/>
@@ -910,7 +905,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:I6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -926,7 +921,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -949,7 +944,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
         <v>5</v>
       </c>
@@ -957,19 +952,19 @@
         <v>4</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>19</v>
@@ -980,7 +975,7 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7">
         <v>0.11</v>
@@ -1013,7 +1008,7 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C8">
         <v>0.11</v>
@@ -1043,10 +1038,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C9">
         <v>0.11</v>
@@ -1079,7 +1074,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10">
         <v>0.22</v>
@@ -1112,7 +1107,7 @@
         <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C11">
         <v>0.22</v>
@@ -1142,10 +1137,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>0.22</v>

</xml_diff>

<commit_message>
Fix electricity mix issues in Ch8
</commit_message>
<xml_diff>
--- a/chapters/ch08-Transportation/datasets/EV data from Hawkins.xlsx
+++ b/chapters/ch08-Transportation/datasets/EV data from Hawkins.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch08-Transportation/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D17DBDA-A25B-2A4F-9C0B-83863F91C0FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7728CE28-A11C-3244-8DAD-CAAA6AAEF422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="24660" windowHeight="13280" xr2:uid="{586E1F71-0C46-D24B-9AE0-864EA31C6727}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="24660" windowHeight="13280" activeTab="1" xr2:uid="{586E1F71-0C46-D24B-9AE0-864EA31C6727}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
   <si>
-    <t>EV-Euro</t>
-  </si>
-  <si>
     <t>GWP</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>ICE-Gas</t>
+  </si>
+  <si>
+    <t>EV-Ren20</t>
   </si>
 </sst>
 </file>
@@ -606,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{545E4E2A-C014-C447-B414-163A5DC3E9E2}">
   <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,23 +638,23 @@
         <v>Battery</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="5" t="str">
         <f>'Hawkins supplemental info'!H6</f>
         <v>Fuel/electricity</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>'Hawkins supplemental info'!C7</f>
@@ -689,10 +689,10 @@
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="str">
         <f>'Hawkins supplemental info'!A8</f>
-        <v>EV-Euro</v>
+        <v>EV-Ren20</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <f>'Hawkins supplemental info'!C8</f>
@@ -730,7 +730,7 @@
         <v>EV-Coal</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <f>'Hawkins supplemental info'!C9</f>
@@ -764,10 +764,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>'Hawkins supplemental info'!C10</f>
@@ -802,10 +802,10 @@
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="str">
         <f>'Hawkins supplemental info'!A11</f>
-        <v>EV-Euro</v>
+        <v>EV-Ren20</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6">
         <f>'Hawkins supplemental info'!C11</f>
@@ -843,7 +843,7 @@
         <v>EV-Coal</v>
       </c>
       <c r="B7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7">
         <f>'Hawkins supplemental info'!C12</f>
@@ -904,8 +904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A13FC51-CB03-F846-84E2-E46C0AEC866C}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -916,12 +916,12 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -929,13 +929,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="C5" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
@@ -946,36 +946,36 @@
     </row>
     <row r="6" spans="1:10" ht="34" x14ac:dyDescent="0.2">
       <c r="C6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7">
         <v>0.11</v>
@@ -1005,10 +1005,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8">
         <v>0.11</v>
@@ -1038,10 +1038,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <v>0.11</v>
@@ -1071,10 +1071,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10">
         <v>0.22</v>
@@ -1104,10 +1104,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <v>0.22</v>
@@ -1137,10 +1137,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
       </c>
       <c r="C12">
         <v>0.22</v>

</xml_diff>